<commit_message>
Clean up query parameters - rest of the files
</commit_message>
<xml_diff>
--- a/Docs/Widgets & layer naming.xlsx
+++ b/Docs/Widgets & layer naming.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5962D62-F1D7-ED45-9442-337205D66123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB7D6B1-B7FA-428D-B46E-AFF4A3255D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16000" xr2:uid="{3444A6CE-5B57-D349-8C15-97E082D49B3C}"/>
+    <workbookView xWindow="495" yWindow="270" windowWidth="24990" windowHeight="14040" activeTab="3" xr2:uid="{3444A6CE-5B57-D349-8C15-97E082D49B3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
+    <sheet name="Widgets" sheetId="1" r:id="rId1"/>
+    <sheet name="Functions" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>faPhotoWidget</t>
   </si>
@@ -342,15 +345,578 @@
   </si>
   <si>
     <t>Used in other queries:</t>
+  </si>
+  <si>
+    <t>setDynamicQueryPars</t>
+  </si>
+  <si>
+    <t>503-505</t>
+  </si>
+  <si>
+    <t>748-750</t>
+  </si>
+  <si>
+    <t>1916-1921</t>
+  </si>
+  <si>
+    <t>openSpeciesTable</t>
+  </si>
+  <si>
+    <t>453-454</t>
+  </si>
+  <si>
+    <t>530-531</t>
+  </si>
+  <si>
+    <t>runQuery</t>
+  </si>
+  <si>
+    <t>1896-1897</t>
+  </si>
+  <si>
+    <t>queryDropDownOptions</t>
+  </si>
+  <si>
+    <t>609-611</t>
+  </si>
+  <si>
+    <t>queryResponseHandler</t>
+  </si>
+  <si>
+    <t>433, 517</t>
+  </si>
+  <si>
+    <t>initFeatureHandling</t>
+  </si>
+  <si>
+    <t>setDisplayLayers</t>
+  </si>
+  <si>
+    <t>81-87</t>
+  </si>
+  <si>
+    <t>1906-1907</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <r>
+      <t>w.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">subLayerName </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>= tableName;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>queryTask</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">url </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>= w.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>mapServiceLayer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">url </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF067D17"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">"/" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>+ w.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>sublayerIDs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>[w.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF871094"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>subLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <t>openSpeciesTable: 1906-1907</t>
+  </si>
+  <si>
+    <r>
+      <t>Should there be a "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staticSubLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", for those widgets/dropdowns where this doesn't change?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">or use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dynamicLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>!customRestService</t>
+  </si>
+  <si>
+    <t>query.</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>outFields</t>
+  </si>
+  <si>
+    <t>orderByFields</t>
+  </si>
+  <si>
+    <t>workingLayerName</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If static, change to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staticSubLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and assign this to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>workingLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in constructor?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>optionalFieldInfo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.tableNames</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maxLayerName</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subLayerName</t>
+    </r>
+  </si>
+  <si>
+    <t>( makeTableHeaderHtml )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Used when setting </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>w.queryTask.url</t>
+    </r>
+  </si>
+  <si>
+    <t>workingLayerName = w.subLayerName</t>
+  </si>
+  <si>
+    <t>workingLayerName = w.maxLayerName</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">... subsequent modifications of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>workingLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> based on filter selections ...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if (w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>else if (w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maxLayerName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>else if (w.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>optionalFieldInfo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>fields &gt; outFields</t>
+  </si>
+  <si>
+    <t>order &gt; orderByFields</t>
+  </si>
+  <si>
+    <t>tableNames &gt; workingLayerName &gt; queryTask.url</t>
+  </si>
+  <si>
+    <t>queryTask.url</t>
+  </si>
+  <si>
+    <t>maxLayerName &gt; workingLayerName &gt; queryTask.url</t>
+  </si>
+  <si>
+    <t>query.where</t>
+  </si>
+  <si>
+    <t>query.outFields</t>
+  </si>
+  <si>
+    <t>query.orderByFields</t>
+  </si>
+  <si>
+    <t>w.queryDistinctCounts</t>
+  </si>
+  <si>
+    <t>w.queryDropDownOptions</t>
+  </si>
+  <si>
+    <t>w.setDynamicQueryPars</t>
+  </si>
+  <si>
+    <t>w.initFeatureHandling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="26">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,16 +975,149 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF7A7A43"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -426,39 +1125,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -770,23 +1636,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BA7BFD-5DEE-A143-A108-8D3641D8E739}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="28.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="30.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19">
+    <row r="1" spans="1:7" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -807,7 +1671,7 @@
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -818,7 +1682,7 @@
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -838,7 +1702,7 @@
       <c r="F5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -852,7 +1716,7 @@
       <c r="F6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -860,10 +1724,10 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -871,10 +1735,10 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -882,10 +1746,10 @@
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -896,7 +1760,7 @@
       <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -904,19 +1768,19 @@
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4"/>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -933,7 +1797,7 @@
       <c r="F13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -958,7 +1822,7 @@
       <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -969,51 +1833,51 @@
       <c r="F16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:7" ht="18.75">
+      <c r="A21" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="F21" s="6" t="s">
+      <c r="B21" s="29"/>
+      <c r="F21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1024,7 +1888,7 @@
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="7" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1035,7 +1899,7 @@
       <c r="F23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1043,7 +1907,7 @@
       <c r="F24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1052,5 +1916,449 @@
     <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002960BB-71A3-457C-AF7B-9A187AE2294A}">
+  <dimension ref="A2:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.125" customWidth="1"/>
+    <col min="9" max="9" width="13.625" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" s="12" customFormat="1">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="14"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9">
+        <v>781</v>
+      </c>
+      <c r="I5" s="9">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="14"/>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="E7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="14"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="9">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="14"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="9">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I14">
+    <sortCondition ref="A3:A14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44121A39-62E4-4242-8592-4D48882BC6C9}">
+  <dimension ref="B3:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="21"/>
+    <col min="2" max="2" width="20.375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="21"/>
+    <col min="4" max="6" width="20.625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="9" style="21"/>
+    <col min="8" max="8" width="11.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="21"/>
+    <col min="10" max="10" width="28.125" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.875" style="21" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" s="19" customFormat="1" ht="18.75">
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="2:11" s="20" customFormat="1">
+      <c r="D4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="H6" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="D8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="D9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="D10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:11" ht="38.25">
+      <c r="D11" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="J12" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="J13" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="31.5">
+      <c r="J14" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="J17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B762A649-2B0B-40D2-988A-BD76AC7617A5}">
+  <dimension ref="B3:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="3" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" s="32" customFormat="1">
+      <c r="B3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="2:6" s="35" customFormat="1">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+    </row>
+    <row r="5" spans="2:6" s="35" customFormat="1">
+      <c r="B5" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="34"/>
+    </row>
+    <row r="6" spans="2:6" s="35" customFormat="1">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="34"/>
+    </row>
+    <row r="7" spans="2:6" s="35" customFormat="1">
+      <c r="B7" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+    </row>
+    <row r="8" spans="2:6" s="35" customFormat="1">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+    </row>
+    <row r="9" spans="2:6" s="35" customFormat="1">
+      <c r="B9" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+    </row>
+    <row r="10" spans="2:6" s="35" customFormat="1">
+      <c r="B10" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="34"/>
+    </row>
+    <row r="11" spans="2:6" s="35" customFormat="1">
+      <c r="B11" s="34"/>
+    </row>
+    <row r="12" spans="2:6" s="35" customFormat="1"/>
+    <row r="13" spans="2:6" s="35" customFormat="1"/>
+    <row r="14" spans="2:6" s="35" customFormat="1"/>
+    <row r="15" spans="2:6" s="35" customFormat="1"/>
+    <row r="16" spans="2:6" s="35" customFormat="1"/>
+    <row r="17" s="35" customFormat="1"/>
+    <row r="18" s="35" customFormat="1"/>
+    <row r="19" s="35" customFormat="1"/>
+    <row r="20" s="35" customFormat="1"/>
+    <row r="21" s="35" customFormat="1"/>
+    <row r="22" s="33" customFormat="1"/>
+    <row r="23" s="33" customFormat="1"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
For offline app testing
</commit_message>
<xml_diff>
--- a/Docs/Widgets & layer naming.xlsx
+++ b/Docs/Widgets & layer naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB7D6B1-B7FA-428D-B46E-AFF4A3255D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4429AA-56E9-42FE-A8B7-2458F92C3A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="495" yWindow="270" windowWidth="24990" windowHeight="14040" activeTab="3" xr2:uid="{3444A6CE-5B57-D349-8C15-97E082D49B3C}"/>
   </bookViews>
@@ -2253,7 +2253,7 @@
   <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>